<commit_message>
Assignment data excel file cleaned, and report completed
</commit_message>
<xml_diff>
--- a/COM1005_Assignment_2021/Assignmentdata.xlsx
+++ b/COM1005_Assignment_2021/Assignmentdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sheffield\COM1005\sem 2\COM1005 FINAL ASSIGNMENT\COM1005_aca20rk\COM1005_Assignment_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB77027-9FF8-47C0-9CED-F01E5355768B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A983C373-4A2B-410C-A446-EBF3685EB4DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{33FD7212-17AC-410A-AE48-3CCC1A054022}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="111">
   <si>
     <t>Efficiency</t>
   </si>
@@ -354,25 +354,19 @@
     <t>(200, 200)</t>
   </si>
   <si>
-    <t>actual 136 bnb</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
-    <t>prob</t>
-  </si>
-  <si>
     <t>A star Euclidean</t>
   </si>
   <si>
-    <t xml:space="preserve">only half </t>
-  </si>
-  <si>
     <t>A star Height + Euclidean</t>
   </si>
   <si>
     <t>A star Manhattan + HEIGHT</t>
+  </si>
+  <si>
+    <t>Costs</t>
   </si>
 </sst>
 </file>
@@ -3374,7 +3368,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$W$3:$W$12,Sheet1!$W$14:$W$38,Sheet1!$W$40:$W$52)</c:f>
+              <c:f>(Sheet1!$U$3:$U$12,Sheet1!$U$14:$U$38,Sheet1!$U$40:$U$52)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
@@ -3527,7 +3521,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$V$3:$V$12,Sheet1!$V$14:$V$38,Sheet1!$V$40:$V$52)</c:f>
+              <c:f>(Sheet1!$T$3:$T$12,Sheet1!$T$14:$T$38,Sheet1!$T$40:$T$52)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
@@ -4125,7 +4119,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$AB$3:$AB$12,Sheet1!$AB$14:$AB$52)</c:f>
+              <c:f>(Sheet1!$X$3:$X$12,Sheet1!$X$14:$X$52)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
@@ -4281,7 +4275,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$AA$3:$AA$12,Sheet1!$AA$14:$AA$52)</c:f>
+              <c:f>(Sheet1!$W$3:$W$12,Sheet1!$W$14:$W$52)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
@@ -8133,7 +8127,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -8171,7 +8165,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -8240,13 +8234,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
@@ -8278,13 +8272,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
@@ -8614,10 +8608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DC1965-235C-4257-99E5-BDF5B0FFBB8E}">
-  <dimension ref="A1:AC99"/>
+  <dimension ref="B1:Y96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8626,43 +8620,48 @@
     <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-      <c r="T1" s="2" t="s">
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="Z1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>67</v>
       </c>
@@ -8672,6 +8671,9 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
@@ -8681,14 +8683,14 @@
       <c r="P2" t="s">
         <v>0</v>
       </c>
-      <c r="V2" t="s">
+      <c r="T2" t="s">
         <v>0</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="W2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -8698,6 +8700,9 @@
       <c r="D3">
         <v>1.420765E-2</v>
       </c>
+      <c r="E3">
+        <v>13</v>
+      </c>
       <c r="H3">
         <v>0.56521739999999998</v>
       </c>
@@ -8713,20 +8718,23 @@
       <c r="P3">
         <v>2.0280811999999999E-2</v>
       </c>
-      <c r="V3">
+      <c r="Q3">
+        <v>14</v>
+      </c>
+      <c r="T3">
         <v>1.9847328000000001E-2</v>
       </c>
+      <c r="U3">
+        <v>13</v>
+      </c>
       <c r="W3">
-        <v>13</v>
-      </c>
-      <c r="AA3">
         <v>0.13</v>
       </c>
-      <c r="AB3">
+      <c r="X3">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -8736,6 +8744,9 @@
       <c r="D4">
         <v>1.5574103000000001E-3</v>
       </c>
+      <c r="E4">
+        <v>218</v>
+      </c>
       <c r="H4">
         <v>6.2324436999999996E-3</v>
       </c>
@@ -8751,20 +8762,23 @@
       <c r="P4">
         <v>2.4456193000000001E-3</v>
       </c>
-      <c r="V4">
+      <c r="Q4">
+        <v>218</v>
+      </c>
+      <c r="T4">
         <v>1.6645371E-3</v>
       </c>
+      <c r="U4">
+        <v>218</v>
+      </c>
       <c r="W4">
-        <v>218</v>
-      </c>
-      <c r="AA4">
         <v>5.2058510000000001E-3</v>
       </c>
-      <c r="AB4">
+      <c r="X4">
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -8774,6 +8788,9 @@
       <c r="D5">
         <v>1.0170667999999999E-3</v>
       </c>
+      <c r="E5">
+        <v>278</v>
+      </c>
       <c r="H5">
         <v>2.7753268000000001E-3</v>
       </c>
@@ -8789,20 +8806,23 @@
       <c r="P5">
         <v>1.1565048000000001E-3</v>
       </c>
-      <c r="V5">
+      <c r="Q5">
+        <v>282</v>
+      </c>
+      <c r="T5">
         <v>1.0427591999999999E-3</v>
       </c>
+      <c r="U5">
+        <v>278</v>
+      </c>
       <c r="W5">
-        <v>278</v>
-      </c>
-      <c r="AA5">
         <v>3.809897E-3</v>
       </c>
-      <c r="AB5">
+      <c r="X5">
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -8812,6 +8832,9 @@
       <c r="D6">
         <v>1.9903625E-3</v>
       </c>
+      <c r="E6">
+        <v>94</v>
+      </c>
       <c r="H6">
         <v>1.5413737E-2</v>
       </c>
@@ -8827,20 +8850,23 @@
       <c r="P6">
         <v>2.8472950000000001E-3</v>
       </c>
-      <c r="V6">
+      <c r="Q6">
+        <v>94</v>
+      </c>
+      <c r="T6">
         <v>2.2862185999999998E-3</v>
       </c>
+      <c r="U6">
+        <v>94</v>
+      </c>
       <c r="W6">
+        <v>2.4245000999999999E-2</v>
+      </c>
+      <c r="X6">
         <v>94</v>
       </c>
-      <c r="AA6">
-        <v>2.4245000999999999E-2</v>
-      </c>
-      <c r="AB6">
-        <v>94</v>
-      </c>
     </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -8850,6 +8876,9 @@
       <c r="D7">
         <v>9.8882630000000004E-4</v>
       </c>
+      <c r="E7">
+        <v>312</v>
+      </c>
       <c r="H7">
         <v>3.8724667E-3</v>
       </c>
@@ -8865,20 +8894,23 @@
       <c r="P7">
         <v>1.2811226E-3</v>
       </c>
-      <c r="V7">
+      <c r="Q7">
+        <v>339</v>
+      </c>
+      <c r="T7">
         <v>1.0455899000000001E-3</v>
       </c>
+      <c r="U7">
+        <v>312</v>
+      </c>
       <c r="W7">
-        <v>312</v>
-      </c>
-      <c r="AA7">
         <v>2.3973940000000002E-3</v>
       </c>
-      <c r="AB7">
+      <c r="X7">
         <v>319</v>
       </c>
     </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -8888,6 +8920,9 @@
       <c r="D8">
         <v>1.4048914E-3</v>
       </c>
+      <c r="E8">
+        <v>326</v>
+      </c>
       <c r="H8">
         <v>2.3955284000000002E-3</v>
       </c>
@@ -8903,20 +8938,23 @@
       <c r="P8">
         <v>2.1208910000000002E-3</v>
       </c>
-      <c r="V8">
+      <c r="Q8">
+        <v>326</v>
+      </c>
+      <c r="T8">
         <v>1.4722913E-3</v>
       </c>
+      <c r="U8">
+        <v>326</v>
+      </c>
       <c r="W8">
+        <v>3.5152435000000001E-3</v>
+      </c>
+      <c r="X8">
         <v>326</v>
       </c>
-      <c r="AA8">
-        <v>3.5152435000000001E-3</v>
-      </c>
-      <c r="AB8">
-        <v>326</v>
-      </c>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -8926,6 +8964,9 @@
       <c r="D9">
         <v>1.3853125E-3</v>
       </c>
+      <c r="E9">
+        <v>234</v>
+      </c>
       <c r="H9">
         <v>6.862061E-3</v>
       </c>
@@ -8941,20 +8982,23 @@
       <c r="P9">
         <v>1.7713284999999999E-3</v>
       </c>
-      <c r="V9">
+      <c r="Q9">
+        <v>234</v>
+      </c>
+      <c r="T9">
         <v>1.4601792000000001E-3</v>
       </c>
+      <c r="U9">
+        <v>234</v>
+      </c>
       <c r="W9">
-        <v>234</v>
-      </c>
-      <c r="AA9">
         <v>1.1794496E-2</v>
       </c>
-      <c r="AB9">
+      <c r="X9">
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -8964,6 +9008,9 @@
       <c r="D10">
         <v>1.7125731E-3</v>
       </c>
+      <c r="E10">
+        <v>81</v>
+      </c>
       <c r="H10">
         <v>8.1892630000000004E-3</v>
       </c>
@@ -8979,20 +9026,23 @@
       <c r="P10">
         <v>3.1181348000000001E-3</v>
       </c>
-      <c r="V10">
+      <c r="Q10">
+        <v>83</v>
+      </c>
+      <c r="T10">
         <v>2.0082563E-3</v>
       </c>
+      <c r="U10">
+        <v>81</v>
+      </c>
       <c r="W10">
-        <v>81</v>
-      </c>
-      <c r="AA10">
         <v>1.323043E-2</v>
       </c>
-      <c r="AB10">
+      <c r="X10">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -9002,6 +9052,9 @@
       <c r="D11">
         <v>1.5493867000000001E-3</v>
       </c>
+      <c r="E11">
+        <v>294</v>
+      </c>
       <c r="H11">
         <v>5.0148726000000003E-3</v>
       </c>
@@ -9017,20 +9070,23 @@
       <c r="P11">
         <v>2.2913625000000001E-3</v>
       </c>
-      <c r="V11">
+      <c r="Q11">
+        <v>294</v>
+      </c>
+      <c r="T11">
         <v>1.6544475E-3</v>
       </c>
+      <c r="U11">
+        <v>294</v>
+      </c>
       <c r="W11">
-        <v>294</v>
-      </c>
-      <c r="AA11">
         <v>5.7266373000000002E-3</v>
       </c>
-      <c r="AB11">
+      <c r="X11">
         <v>354</v>
       </c>
     </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>69</v>
       </c>
@@ -9040,6 +9096,9 @@
       <c r="D12">
         <v>3.8109757000000001E-3</v>
       </c>
+      <c r="E12">
+        <v>54</v>
+      </c>
       <c r="H12">
         <v>4.3171115000000003E-2</v>
       </c>
@@ -9055,20 +9114,23 @@
       <c r="P12">
         <v>1.2334604000000001E-2</v>
       </c>
-      <c r="V12">
+      <c r="Q12">
+        <v>54</v>
+      </c>
+      <c r="T12">
         <v>4.6519496999999996E-3</v>
       </c>
+      <c r="U12">
+        <v>54</v>
+      </c>
       <c r="W12">
-        <v>54</v>
-      </c>
-      <c r="AA12">
         <v>0.47826087</v>
       </c>
-      <c r="AB12">
+      <c r="X12">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -9078,6 +9140,9 @@
       <c r="D13">
         <v>2.5830257999999998E-2</v>
       </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
       <c r="H13">
         <v>0.16279070000000001</v>
       </c>
@@ -9093,20 +9158,23 @@
       <c r="P13">
         <v>0.5</v>
       </c>
-      <c r="V13">
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="T13">
         <v>3.8043476999999999E-2</v>
       </c>
+      <c r="U13">
+        <v>10</v>
+      </c>
       <c r="W13">
+        <v>0.77777777777000001</v>
+      </c>
+      <c r="X13">
         <v>10</v>
       </c>
-      <c r="AA13">
-        <v>0.77777777777000001</v>
-      </c>
-      <c r="AB13">
-        <v>10</v>
-      </c>
     </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>70</v>
       </c>
@@ -9116,6 +9184,9 @@
       <c r="D14">
         <v>1.7446649E-3</v>
       </c>
+      <c r="E14">
+        <v>152</v>
+      </c>
       <c r="H14">
         <v>9.5288909999999994E-3</v>
       </c>
@@ -9131,20 +9202,23 @@
       <c r="P14">
         <v>2.3413063000000001E-3</v>
       </c>
-      <c r="V14">
+      <c r="Q14">
+        <v>152</v>
+      </c>
+      <c r="T14">
         <v>1.9166488E-3</v>
       </c>
+      <c r="U14">
+        <v>152</v>
+      </c>
       <c r="W14">
-        <v>152</v>
-      </c>
-      <c r="AA14">
         <v>1.8129078999999999E-2</v>
       </c>
-      <c r="AB14">
+      <c r="X14">
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -9154,6 +9228,9 @@
       <c r="D15">
         <v>2.2308438E-3</v>
       </c>
+      <c r="E15">
+        <v>134</v>
+      </c>
       <c r="H15">
         <v>6.7821599999999998E-3</v>
       </c>
@@ -9169,20 +9246,23 @@
       <c r="P15">
         <v>3.0011479999999999E-3</v>
       </c>
-      <c r="V15">
+      <c r="Q15">
+        <v>134</v>
+      </c>
+      <c r="T15">
         <v>2.286396E-3</v>
       </c>
+      <c r="U15">
+        <v>134</v>
+      </c>
       <c r="W15">
+        <v>6.6570185000000004E-2</v>
+      </c>
+      <c r="X15">
         <v>134</v>
       </c>
-      <c r="AA15">
-        <v>6.6570185000000004E-2</v>
-      </c>
-      <c r="AB15">
-        <v>134</v>
-      </c>
     </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -9192,6 +9272,9 @@
       <c r="D16">
         <v>5.8837654000000001E-3</v>
       </c>
+      <c r="E16">
+        <v>75</v>
+      </c>
       <c r="H16">
         <v>1.2586694000000001E-2</v>
       </c>
@@ -9207,20 +9290,23 @@
       <c r="P16">
         <v>9.2926229999999999E-3</v>
       </c>
-      <c r="V16">
+      <c r="Q16">
+        <v>75</v>
+      </c>
+      <c r="T16">
         <v>6.1089639999999997E-3</v>
       </c>
+      <c r="U16">
+        <v>75</v>
+      </c>
       <c r="W16">
+        <v>1.9036517999999999E-2</v>
+      </c>
+      <c r="X16">
         <v>75</v>
       </c>
-      <c r="AA16">
-        <v>1.9036517999999999E-2</v>
-      </c>
-      <c r="AB16">
-        <v>75</v>
-      </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -9230,6 +9316,9 @@
       <c r="D17">
         <v>1.5172136000000001E-3</v>
       </c>
+      <c r="E17">
+        <v>143</v>
+      </c>
       <c r="H17">
         <v>2.3730587000000001E-2</v>
       </c>
@@ -9245,20 +9334,23 @@
       <c r="P17">
         <v>3.230634E-3</v>
       </c>
-      <c r="V17">
+      <c r="Q17">
+        <v>54</v>
+      </c>
+      <c r="T17">
         <v>1.7529613E-3</v>
       </c>
+      <c r="U17">
+        <v>143</v>
+      </c>
       <c r="W17">
+        <v>0.16171224000000001</v>
+      </c>
+      <c r="X17">
         <v>143</v>
       </c>
-      <c r="AA17">
-        <v>0.16171224000000001</v>
-      </c>
-      <c r="AB17">
-        <v>143</v>
-      </c>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>72</v>
       </c>
@@ -9268,6 +9360,9 @@
       <c r="D18">
         <v>2.5860042999999999E-3</v>
       </c>
+      <c r="E18">
+        <v>102</v>
+      </c>
       <c r="H18">
         <v>8.4507049999999993E-3</v>
       </c>
@@ -9283,20 +9378,23 @@
       <c r="P18">
         <v>4.0077725000000003E-3</v>
       </c>
-      <c r="V18">
+      <c r="Q18">
+        <v>102</v>
+      </c>
+      <c r="T18">
         <v>2.7464526000000001E-3</v>
       </c>
+      <c r="U18">
+        <v>102</v>
+      </c>
       <c r="W18">
+        <v>2.9596412999999998E-2</v>
+      </c>
+      <c r="X18">
         <v>102</v>
       </c>
-      <c r="AA18">
-        <v>2.9596412999999998E-2</v>
-      </c>
-      <c r="AB18">
-        <v>102</v>
-      </c>
     </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -9306,6 +9404,9 @@
       <c r="D19">
         <v>5.1396135000000001E-3</v>
       </c>
+      <c r="E19">
+        <v>68</v>
+      </c>
       <c r="H19">
         <v>8.2920789999999994E-2</v>
       </c>
@@ -9321,20 +9422,23 @@
       <c r="P19">
         <v>0.1231165</v>
       </c>
-      <c r="V19">
+      <c r="Q19">
+        <v>68</v>
+      </c>
+      <c r="T19">
         <v>5.8633060000000004E-3</v>
       </c>
+      <c r="U19">
+        <v>68</v>
+      </c>
       <c r="W19">
-        <v>68</v>
-      </c>
-      <c r="AA19">
         <v>0.25093632999999999</v>
       </c>
-      <c r="AB19">
+      <c r="X19">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>73</v>
       </c>
@@ -9344,6 +9448,9 @@
       <c r="D20">
         <v>1.6922209E-3</v>
       </c>
+      <c r="E20">
+        <v>140</v>
+      </c>
       <c r="H20">
         <v>1.1495587E-2</v>
       </c>
@@ -9359,20 +9466,23 @@
       <c r="P20">
         <v>2.3628249999999998E-3</v>
       </c>
-      <c r="V20">
+      <c r="Q20">
+        <v>140</v>
+      </c>
+      <c r="T20">
         <v>1.8203548E-3</v>
       </c>
+      <c r="U20">
+        <v>140</v>
+      </c>
       <c r="W20">
-        <v>140</v>
-      </c>
-      <c r="AA20">
         <v>1.1490251E-2</v>
       </c>
-      <c r="AB20">
+      <c r="X20">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>74</v>
       </c>
@@ -9403,20 +9513,20 @@
       <c r="Q21">
         <v>110</v>
       </c>
-      <c r="V21">
+      <c r="T21">
         <v>1.4329913999999999E-3</v>
       </c>
+      <c r="U21">
+        <v>110</v>
+      </c>
       <c r="W21">
-        <v>110</v>
-      </c>
-      <c r="AA21">
         <v>7.4702889999999994E-2</v>
       </c>
-      <c r="AB21">
+      <c r="X21">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -9447,20 +9557,20 @@
       <c r="Q22">
         <v>255</v>
       </c>
-      <c r="V22">
+      <c r="T22">
         <v>5.0132424000000004E-3</v>
       </c>
+      <c r="U22">
+        <v>59</v>
+      </c>
       <c r="W22">
-        <v>59</v>
-      </c>
-      <c r="AA22">
         <v>2.9608939000000001E-2</v>
       </c>
-      <c r="AB22">
+      <c r="X22">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>76</v>
       </c>
@@ -9491,20 +9601,20 @@
       <c r="Q23">
         <v>355</v>
       </c>
-      <c r="V23">
+      <c r="T23">
         <v>1.499142E-3</v>
       </c>
+      <c r="U23">
+        <v>141</v>
+      </c>
       <c r="W23">
-        <v>141</v>
-      </c>
-      <c r="AA23">
         <v>2.1699347000000001E-2</v>
       </c>
-      <c r="AB23">
+      <c r="X23">
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -9535,20 +9645,20 @@
       <c r="Q24">
         <v>233</v>
       </c>
-      <c r="V24">
+      <c r="T24">
         <v>1.2101654E-2</v>
       </c>
+      <c r="U24">
+        <v>29</v>
+      </c>
       <c r="W24">
+        <v>0.48387095000000002</v>
+      </c>
+      <c r="X24">
         <v>29</v>
       </c>
-      <c r="AA24">
-        <v>0.48387095000000002</v>
-      </c>
-      <c r="AB24">
-        <v>29</v>
-      </c>
     </row>
-    <row r="25" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>77</v>
       </c>
@@ -9579,20 +9689,20 @@
       <c r="Q25">
         <v>133</v>
       </c>
-      <c r="V25">
+      <c r="T25">
         <v>1.5823019E-3</v>
       </c>
+      <c r="U25">
+        <v>133</v>
+      </c>
       <c r="W25">
-        <v>133</v>
-      </c>
-      <c r="AA25">
         <v>1.2274959E-2</v>
       </c>
-      <c r="AB25">
+      <c r="X25">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>78</v>
       </c>
@@ -9623,20 +9733,20 @@
       <c r="Q26">
         <v>275</v>
       </c>
-      <c r="V26">
+      <c r="T26">
         <v>1.6094979E-3</v>
       </c>
+      <c r="U26">
+        <v>275</v>
+      </c>
       <c r="W26">
-        <v>275</v>
-      </c>
-      <c r="AA26">
         <v>4.3481600000000002E-3</v>
       </c>
-      <c r="AB26">
+      <c r="X26">
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -9667,20 +9777,20 @@
       <c r="Q27">
         <v>70</v>
       </c>
-      <c r="V27">
+      <c r="T27">
         <v>3.6819372000000002E-3</v>
       </c>
+      <c r="U27">
+        <v>70</v>
+      </c>
       <c r="W27">
+        <v>1.7918676000000001E-2</v>
+      </c>
+      <c r="X27">
         <v>70</v>
       </c>
-      <c r="AA27">
-        <v>1.7918676000000001E-2</v>
-      </c>
-      <c r="AB27">
-        <v>70</v>
-      </c>
     </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>46</v>
       </c>
@@ -9711,20 +9821,20 @@
       <c r="Q28">
         <v>102</v>
       </c>
-      <c r="V28">
+      <c r="T28">
         <v>4.9093994000000002E-3</v>
       </c>
+      <c r="U28">
+        <v>102</v>
+      </c>
       <c r="W28">
+        <v>1.3732833999999999E-2</v>
+      </c>
+      <c r="X28">
         <v>102</v>
       </c>
-      <c r="AA28">
-        <v>1.3732833999999999E-2</v>
-      </c>
-      <c r="AB28">
-        <v>102</v>
-      </c>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>47</v>
       </c>
@@ -9755,20 +9865,20 @@
       <c r="Q29">
         <v>114</v>
       </c>
-      <c r="V29">
+      <c r="T29">
         <v>1.8230389E-3</v>
       </c>
+      <c r="U29">
+        <v>114</v>
+      </c>
       <c r="W29">
-        <v>114</v>
-      </c>
-      <c r="AA29">
         <v>1.8515123000000001E-2</v>
       </c>
-      <c r="AB29">
+      <c r="X29">
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>48</v>
       </c>
@@ -9799,23 +9909,20 @@
       <c r="Q30">
         <v>292</v>
       </c>
-      <c r="R30" t="s">
-        <v>106</v>
-      </c>
-      <c r="V30">
+      <c r="T30">
         <v>1.1439753000000001E-3</v>
       </c>
+      <c r="U30">
+        <v>136</v>
+      </c>
       <c r="W30">
-        <v>136</v>
-      </c>
-      <c r="AA30">
         <v>2.8614457999999999E-2</v>
       </c>
-      <c r="AB30">
+      <c r="X30">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>49</v>
       </c>
@@ -9846,20 +9953,20 @@
       <c r="Q31">
         <v>201</v>
       </c>
-      <c r="V31">
+      <c r="T31">
         <v>9.9549100000000004E-4</v>
       </c>
+      <c r="U31">
+        <v>201</v>
+      </c>
       <c r="W31">
-        <v>201</v>
-      </c>
-      <c r="AA31">
         <v>1.2644776999999999E-2</v>
       </c>
-      <c r="AB31">
+      <c r="X31">
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>50</v>
       </c>
@@ -9890,23 +9997,20 @@
       <c r="Q32">
         <v>253</v>
       </c>
-      <c r="R32">
+      <c r="T32">
+        <v>1.4673931E-3</v>
+      </c>
+      <c r="U32">
         <v>248</v>
       </c>
-      <c r="V32">
-        <v>1.4673931E-3</v>
-      </c>
       <c r="W32">
-        <v>248</v>
-      </c>
-      <c r="AA32">
         <v>3.3688499E-3</v>
       </c>
-      <c r="AB32">
+      <c r="X32">
         <v>256</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>85</v>
       </c>
@@ -9937,20 +10041,20 @@
       <c r="Q33">
         <v>120</v>
       </c>
-      <c r="V33">
+      <c r="T33">
         <v>1.2299843E-3</v>
       </c>
+      <c r="U33">
+        <v>120</v>
+      </c>
       <c r="W33">
-        <v>120</v>
-      </c>
-      <c r="AA33">
         <v>1.1223828999999999E-2</v>
       </c>
-      <c r="AB33">
+      <c r="X33">
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>86</v>
       </c>
@@ -9981,20 +10085,20 @@
       <c r="Q34">
         <v>193</v>
       </c>
-      <c r="V34">
+      <c r="T34">
         <v>1.1401196E-3</v>
       </c>
+      <c r="U34">
+        <v>193</v>
+      </c>
       <c r="W34">
-        <v>193</v>
-      </c>
-      <c r="AA34">
         <v>4.2450439999999999E-3</v>
       </c>
-      <c r="AB34">
+      <c r="X34">
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>51</v>
       </c>
@@ -10025,20 +10129,20 @@
       <c r="Q35">
         <v>54</v>
       </c>
-      <c r="V35">
+      <c r="T35">
         <v>2.9708853E-3</v>
       </c>
+      <c r="U35">
+        <v>54</v>
+      </c>
       <c r="W35">
+        <v>2.0424837000000001E-2</v>
+      </c>
+      <c r="X35">
         <v>54</v>
       </c>
-      <c r="AA35">
-        <v>2.0424837000000001E-2</v>
-      </c>
-      <c r="AB35">
-        <v>54</v>
-      </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>52</v>
       </c>
@@ -10069,20 +10173,20 @@
       <c r="Q36">
         <v>80</v>
       </c>
-      <c r="V36">
+      <c r="T36">
         <v>4.5076500000000002E-3</v>
       </c>
+      <c r="U36">
+        <v>80</v>
+      </c>
       <c r="W36">
-        <v>80</v>
-      </c>
-      <c r="AA36">
         <v>7.2895269999999998E-2</v>
       </c>
-      <c r="AB36">
+      <c r="X36">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>53</v>
       </c>
@@ -10113,23 +10217,20 @@
       <c r="Q37">
         <v>86</v>
       </c>
-      <c r="R37">
-        <v>94</v>
-      </c>
-      <c r="V37">
+      <c r="T37">
         <v>2.6622717000000001E-3</v>
       </c>
+      <c r="U37">
+        <v>86</v>
+      </c>
       <c r="W37">
+        <v>1.8329939E-2</v>
+      </c>
+      <c r="X37">
         <v>86</v>
       </c>
-      <c r="AA37">
-        <v>1.8329939E-2</v>
-      </c>
-      <c r="AB37">
-        <v>86</v>
-      </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>54</v>
       </c>
@@ -10160,23 +10261,20 @@
       <c r="Q38">
         <v>94</v>
       </c>
-      <c r="R38">
-        <v>86</v>
-      </c>
-      <c r="V38">
+      <c r="T38">
         <v>3.8567085000000001E-3</v>
       </c>
+      <c r="U38">
+        <v>94</v>
+      </c>
       <c r="W38">
+        <v>4.0404040400000001E-2</v>
+      </c>
+      <c r="X38">
         <v>94</v>
       </c>
-      <c r="AA38">
-        <v>4.0404040400000001E-2</v>
-      </c>
-      <c r="AB38">
-        <v>94</v>
-      </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>55</v>
       </c>
@@ -10195,23 +10293,35 @@
       <c r="I39">
         <v>130</v>
       </c>
+      <c r="L39">
+        <v>3.7882829999999999E-3</v>
+      </c>
+      <c r="M39">
+        <v>130</v>
+      </c>
       <c r="P39">
         <v>4.7882829999999999E-3</v>
       </c>
       <c r="Q39">
         <v>130</v>
       </c>
-      <c r="AA39">
+      <c r="T39">
+        <v>1.0420923E-2</v>
+      </c>
+      <c r="U39">
+        <v>130</v>
+      </c>
+      <c r="W39">
         <v>1.7302798000000001E-2</v>
       </c>
-      <c r="AB39">
+      <c r="X39">
         <v>142</v>
       </c>
-      <c r="AC39" t="s">
-        <v>107</v>
+      <c r="Y39" t="s">
+        <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>90</v>
       </c>
@@ -10242,20 +10352,20 @@
       <c r="Q40">
         <v>62</v>
       </c>
-      <c r="V40">
+      <c r="T40">
         <v>1.3287775E-2</v>
       </c>
+      <c r="U40">
+        <v>62</v>
+      </c>
       <c r="W40">
+        <v>3.0068729999999998E-2</v>
+      </c>
+      <c r="X40">
         <v>62</v>
       </c>
-      <c r="AA40">
-        <v>3.0068729999999998E-2</v>
-      </c>
-      <c r="AB40">
-        <v>62</v>
-      </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>56</v>
       </c>
@@ -10286,20 +10396,20 @@
       <c r="Q41">
         <v>42</v>
       </c>
-      <c r="V41">
+      <c r="T41">
         <v>1.0411244E-2</v>
       </c>
+      <c r="U41">
+        <v>42</v>
+      </c>
       <c r="W41">
+        <v>8.0482899999999996E-2</v>
+      </c>
+      <c r="X41">
         <v>42</v>
       </c>
-      <c r="AA41">
-        <v>8.0482899999999996E-2</v>
-      </c>
-      <c r="AB41">
-        <v>42</v>
-      </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>57</v>
       </c>
@@ -10330,20 +10440,20 @@
       <c r="Q42">
         <v>105</v>
       </c>
-      <c r="V42">
+      <c r="T42">
         <v>1.4224750999999999E-3</v>
       </c>
+      <c r="U42">
+        <v>105</v>
+      </c>
       <c r="W42">
+        <v>1.3544018E-2</v>
+      </c>
+      <c r="X42">
         <v>105</v>
       </c>
-      <c r="AA42">
-        <v>1.3544018E-2</v>
-      </c>
-      <c r="AB42">
-        <v>105</v>
-      </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>93</v>
       </c>
@@ -10374,20 +10484,20 @@
       <c r="Q43">
         <v>35</v>
       </c>
-      <c r="V43">
+      <c r="T43">
         <v>8.9450139999999994E-3</v>
       </c>
+      <c r="U43">
+        <v>35</v>
+      </c>
       <c r="W43">
+        <v>0.13545816999999999</v>
+      </c>
+      <c r="X43">
         <v>35</v>
       </c>
-      <c r="AA43">
-        <v>0.13545816999999999</v>
-      </c>
-      <c r="AB43">
-        <v>35</v>
-      </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>63</v>
       </c>
@@ -10418,20 +10528,20 @@
       <c r="Q44">
         <v>46</v>
       </c>
-      <c r="V44">
+      <c r="T44">
         <v>3.2679739999999999E-3</v>
       </c>
+      <c r="U44">
+        <v>46</v>
+      </c>
       <c r="W44">
+        <v>0.108571425</v>
+      </c>
+      <c r="X44">
         <v>46</v>
       </c>
-      <c r="AA44">
-        <v>0.108571425</v>
-      </c>
-      <c r="AB44">
-        <v>46</v>
-      </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>95</v>
       </c>
@@ -10462,26 +10572,20 @@
       <c r="Q45">
         <v>40</v>
       </c>
-      <c r="R45">
+      <c r="T45">
+        <v>4.8633627999999998E-3</v>
+      </c>
+      <c r="U45">
         <v>34</v>
       </c>
-      <c r="V45">
-        <v>4.8633627999999998E-3</v>
-      </c>
       <c r="W45">
+        <v>3.0259365E-2</v>
+      </c>
+      <c r="X45">
         <v>34</v>
       </c>
-      <c r="AA45">
-        <v>3.0259365E-2</v>
-      </c>
-      <c r="AB45">
-        <v>34</v>
-      </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>107</v>
-      </c>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>64</v>
       </c>
@@ -10506,29 +10610,26 @@
       <c r="M46">
         <v>130</v>
       </c>
-      <c r="N46" t="s">
-        <v>108</v>
-      </c>
       <c r="P46">
         <v>1.4977974E-2</v>
       </c>
       <c r="Q46">
         <v>35</v>
       </c>
-      <c r="V46">
+      <c r="T46">
         <v>2.1388132999999999E-3</v>
       </c>
+      <c r="U46">
+        <v>130</v>
+      </c>
       <c r="W46">
-        <v>130</v>
-      </c>
-      <c r="AA46">
         <v>1.7302798000000001E-2</v>
       </c>
-      <c r="AB46">
+      <c r="X46">
         <v>142</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>97</v>
       </c>
@@ -10559,20 +10660,20 @@
       <c r="Q47">
         <v>66</v>
       </c>
-      <c r="V47">
+      <c r="T47">
         <v>3.3326497999999999E-3</v>
       </c>
+      <c r="U47">
+        <v>66</v>
+      </c>
       <c r="W47">
-        <v>66</v>
-      </c>
-      <c r="AA47">
         <v>0.17060368000000001</v>
       </c>
-      <c r="AB47">
+      <c r="X47">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>99</v>
       </c>
@@ -10603,20 +10704,20 @@
       <c r="Q48">
         <v>65</v>
       </c>
-      <c r="V48">
+      <c r="T48">
         <v>2.8653296E-3</v>
       </c>
+      <c r="U48">
+        <v>65</v>
+      </c>
       <c r="W48">
-        <v>65</v>
-      </c>
-      <c r="AA48">
         <v>4.4375642999999999E-2</v>
       </c>
-      <c r="AB48">
+      <c r="X48">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>101</v>
       </c>
@@ -10647,20 +10748,20 @@
       <c r="Q49">
         <v>75</v>
       </c>
-      <c r="V49">
+      <c r="T49">
         <v>2.9993289999999998E-3</v>
       </c>
+      <c r="U49">
+        <v>75</v>
+      </c>
       <c r="W49">
-        <v>75</v>
-      </c>
-      <c r="AA49">
         <v>0.45508979999999999</v>
       </c>
-      <c r="AB49">
+      <c r="X49">
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>65</v>
       </c>
@@ -10691,20 +10792,20 @@
       <c r="Q50">
         <v>80</v>
       </c>
-      <c r="V50">
+      <c r="T50">
         <v>2.0491801999999999E-3</v>
       </c>
+      <c r="U50">
+        <v>80</v>
+      </c>
       <c r="W50">
+        <v>1.9955654E-2</v>
+      </c>
+      <c r="X50">
         <v>80</v>
       </c>
-      <c r="AA50">
-        <v>1.9955654E-2</v>
-      </c>
-      <c r="AB50">
-        <v>80</v>
-      </c>
     </row>
-    <row r="51" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>66</v>
       </c>
@@ -10735,23 +10836,20 @@
       <c r="Q51">
         <v>45</v>
       </c>
-      <c r="R51">
+      <c r="T51">
+        <v>6.2052505000000004E-3</v>
+      </c>
+      <c r="U51">
         <v>45</v>
       </c>
-      <c r="V51">
-        <v>6.2052505000000004E-3</v>
-      </c>
       <c r="W51">
-        <v>45</v>
-      </c>
-      <c r="AA51">
         <v>0.10512129000000001</v>
       </c>
-      <c r="AB51">
+      <c r="X51">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>104</v>
       </c>
@@ -10782,23 +10880,20 @@
       <c r="Q52">
         <v>569</v>
       </c>
-      <c r="R52">
+      <c r="T52">
+        <v>1.8106699000000001E-3</v>
+      </c>
+      <c r="U52">
         <v>568</v>
       </c>
-      <c r="V52">
-        <v>1.8106699000000001E-3</v>
-      </c>
       <c r="W52">
-        <v>568</v>
-      </c>
-      <c r="AA52">
         <v>2.8855980000000001E-3</v>
       </c>
-      <c r="AB52">
+      <c r="X52">
         <v>599</v>
       </c>
     </row>
-    <row r="53" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:24" x14ac:dyDescent="0.35">
       <c r="D53" s="1">
         <f>AVERAGE(D3:D52)</f>
         <v>3.4942246660000006E-3</v>
@@ -10809,371 +10904,32 @@
       </c>
       <c r="L53" s="1">
         <f>AVERAGE(L3:L52)</f>
-        <v>1.0362525014489796E-2</v>
+        <v>1.0231040174199998E-2</v>
       </c>
       <c r="P53" s="1">
         <f>AVERAGE(P3:P52)</f>
         <v>1.8385557853999996E-2</v>
       </c>
-      <c r="V53" s="1">
-        <f>AVERAGE(V3:V52)</f>
-        <v>4.3856911918367337E-3</v>
-      </c>
-      <c r="AA53">
-        <f>AVERAGE(AA3:AA52)</f>
+      <c r="T53" s="1">
+        <f>AVERAGE(T3:T52)</f>
+        <v>4.5063958279999983E-3</v>
+      </c>
+      <c r="W53">
+        <f>AVERAGE(W3:W52)</f>
         <v>8.2665588097399989E-2</v>
       </c>
     </row>
-    <row r="89" spans="2:28" x14ac:dyDescent="0.35">
-      <c r="B89" t="s">
-        <v>74</v>
-      </c>
-      <c r="C89" t="s">
-        <v>37</v>
-      </c>
-      <c r="D89">
-        <v>1.2677579999999999E-3</v>
-      </c>
-      <c r="E89">
-        <v>110</v>
-      </c>
-      <c r="H89">
-        <v>4.076339E-3</v>
-      </c>
-      <c r="I89">
-        <v>110</v>
-      </c>
-      <c r="L89">
-        <v>6.869633E-3</v>
-      </c>
-      <c r="M89">
-        <v>110</v>
-      </c>
-      <c r="P89">
-        <v>8.5122849999999996E-3</v>
-      </c>
-      <c r="Q89">
-        <v>110</v>
-      </c>
-      <c r="V89">
-        <v>1.4329913999999999E-3</v>
-      </c>
-      <c r="W89">
-        <v>110</v>
-      </c>
-      <c r="AA89">
-        <v>7.4702889999999994E-2</v>
-      </c>
-      <c r="AB89">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="90" spans="2:28" x14ac:dyDescent="0.35">
-      <c r="B90" t="s">
-        <v>50</v>
-      </c>
-      <c r="C90" t="s">
-        <v>83</v>
-      </c>
-      <c r="D90">
-        <v>1.3944438E-3</v>
-      </c>
-      <c r="E90">
-        <v>248</v>
-      </c>
-      <c r="H90">
-        <v>2.6662257000000002E-3</v>
-      </c>
-      <c r="I90">
-        <v>248</v>
-      </c>
-      <c r="L90">
-        <v>1.8171743000000001E-3</v>
-      </c>
-      <c r="M90">
-        <v>253</v>
-      </c>
-      <c r="P90">
-        <v>1.887045E-3</v>
-      </c>
-      <c r="Q90">
-        <v>253</v>
-      </c>
-      <c r="V90">
-        <v>1.4673931E-3</v>
-      </c>
-      <c r="W90">
-        <v>248</v>
-      </c>
-      <c r="AA90">
-        <v>3.3688499E-3</v>
-      </c>
-      <c r="AB90">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="91" spans="2:28" x14ac:dyDescent="0.35">
-      <c r="B91" t="s">
-        <v>85</v>
-      </c>
-      <c r="C91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D91">
-        <v>1.0984764000000001E-3</v>
-      </c>
-      <c r="E91">
-        <v>120</v>
-      </c>
-      <c r="H91">
-        <v>4.5288274999999998E-3</v>
-      </c>
-      <c r="I91">
-        <v>120</v>
-      </c>
-      <c r="L91">
-        <v>2.1997546000000002E-3</v>
-      </c>
-      <c r="M91">
-        <v>120</v>
-      </c>
-      <c r="P91">
-        <v>2.6344033000000001E-3</v>
-      </c>
-      <c r="Q91">
-        <v>120</v>
-      </c>
-      <c r="V91">
-        <v>1.2299843E-3</v>
-      </c>
-      <c r="W91">
-        <v>120</v>
-      </c>
-      <c r="AA91">
-        <v>1.1223828999999999E-2</v>
-      </c>
-      <c r="AB91">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="92" spans="2:28" x14ac:dyDescent="0.35">
-      <c r="B92" t="s">
-        <v>86</v>
-      </c>
-      <c r="C92" t="s">
-        <v>87</v>
-      </c>
-      <c r="D92">
-        <v>1.1017916E-3</v>
-      </c>
-      <c r="E92">
-        <v>193</v>
-      </c>
-      <c r="H92">
-        <v>4.5898603E-3</v>
-      </c>
-      <c r="I92">
-        <v>193</v>
-      </c>
-      <c r="L92">
-        <v>1.1677486999999999E-3</v>
-      </c>
-      <c r="M92">
-        <v>198</v>
-      </c>
-      <c r="P92">
-        <v>1.2098744E-3</v>
-      </c>
-      <c r="Q92">
-        <v>193</v>
-      </c>
-      <c r="V92">
-        <v>1.1401196E-3</v>
-      </c>
-      <c r="W92">
-        <v>193</v>
-      </c>
-      <c r="AA92">
-        <v>4.2450439999999999E-3</v>
-      </c>
-      <c r="AB92">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="93" spans="2:28" x14ac:dyDescent="0.35">
-      <c r="B93" t="s">
-        <v>51</v>
-      </c>
-      <c r="C93" t="s">
-        <v>44</v>
-      </c>
-      <c r="D93">
-        <v>2.5767882000000001E-3</v>
-      </c>
-      <c r="E93">
-        <v>54</v>
-      </c>
-      <c r="H93">
-        <v>1.5451174E-2</v>
-      </c>
-      <c r="I93">
-        <v>54</v>
-      </c>
-      <c r="L93">
-        <v>4.8412085000000002E-3</v>
-      </c>
-      <c r="M93">
-        <v>54</v>
-      </c>
-      <c r="P93">
-        <v>5.5236410000000001E-3</v>
-      </c>
-      <c r="Q93">
-        <v>54</v>
-      </c>
-      <c r="V93">
-        <v>2.9708853E-3</v>
-      </c>
-      <c r="W93">
-        <v>54</v>
-      </c>
-      <c r="AA93">
-        <v>2.0424837000000001E-2</v>
-      </c>
-      <c r="AB93">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="94" spans="2:28" x14ac:dyDescent="0.35">
-      <c r="B94" t="s">
-        <v>66</v>
-      </c>
-      <c r="C94" t="s">
-        <v>103</v>
-      </c>
-      <c r="D94">
-        <v>5.243345E-3</v>
-      </c>
-      <c r="E94">
-        <v>45</v>
-      </c>
-      <c r="H94">
-        <v>2.895323E-2</v>
-      </c>
-      <c r="I94">
-        <v>45</v>
-      </c>
-      <c r="L94">
-        <v>1.2678804E-2</v>
-      </c>
-      <c r="M94">
-        <v>45</v>
-      </c>
-      <c r="P94">
-        <v>1.5931372999999999E-2</v>
-      </c>
-      <c r="Q94">
-        <v>45</v>
-      </c>
-      <c r="V94">
-        <v>6.2052505000000004E-3</v>
-      </c>
-      <c r="W94">
-        <v>45</v>
-      </c>
-      <c r="AA94">
-        <v>0.10512129000000001</v>
-      </c>
-      <c r="AB94">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="95" spans="2:28" x14ac:dyDescent="0.35">
-      <c r="B95" t="s">
-        <v>104</v>
-      </c>
-      <c r="C95" t="s">
-        <v>105</v>
-      </c>
-      <c r="D95">
-        <v>1.7858256E-3</v>
-      </c>
-      <c r="E95">
-        <v>568</v>
-      </c>
-      <c r="H95">
-        <v>3.0883450000000002E-3</v>
-      </c>
-      <c r="I95">
-        <v>568</v>
-      </c>
-      <c r="L95">
-        <v>1.9538571099999998E-3</v>
-      </c>
-      <c r="M95">
-        <v>569</v>
-      </c>
-      <c r="P95">
-        <v>2.0116079999999998E-3</v>
-      </c>
-      <c r="Q95">
-        <v>569</v>
-      </c>
-      <c r="V95">
-        <v>1.8106699000000001E-3</v>
-      </c>
-      <c r="W95">
-        <v>568</v>
-      </c>
-      <c r="AA95">
-        <v>2.8855980000000001E-3</v>
-      </c>
-      <c r="AB95">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="96" spans="2:28" x14ac:dyDescent="0.35">
-      <c r="D96">
-        <v>3.4942246660000006E-3</v>
-      </c>
-      <c r="H96">
-        <v>4.0833194194000007E-2</v>
-      </c>
-      <c r="L96" s="1">
-        <v>1.0362525014489796E-2</v>
-      </c>
-      <c r="P96">
-        <v>1.8385557853999996E-2</v>
-      </c>
-      <c r="V96">
-        <v>4.3856911918367337E-3</v>
-      </c>
-      <c r="AA96">
-        <v>8.2665588097399989E-2</v>
-      </c>
-    </row>
-    <row r="98" spans="7:15" x14ac:dyDescent="0.35">
-      <c r="O98">
-        <f>AA96/D96</f>
-        <v>23.657777046154013</v>
-      </c>
-    </row>
-    <row r="99" spans="7:15" x14ac:dyDescent="0.35">
-      <c r="G99" t="s">
-        <v>110</v>
-      </c>
-      <c r="O99">
-        <v>1</v>
-      </c>
+    <row r="96" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L96" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>